<commit_message>
add possibility to except columns
</commit_message>
<xml_diff>
--- a/tests/Feature/JoinBelongsToSelectTest/joinable_dummies.xlsx
+++ b/tests/Feature/JoinBelongsToSelectTest/joinable_dummies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -31,7 +31,13 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">joinable_relation.foreign_field</t>
+    <t xml:space="preserve">joinable_select_relation.foreign_field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joinable_except_relation.foreign_field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joinable_both_relation.foreign_field</t>
   </si>
   <si>
     <t xml:space="preserve">title 1</t>
@@ -178,10 +184,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -206,19 +212,31 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,13 +244,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,13 +264,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>